<commit_message>
fig formatting & supplemental tables
revised chapter Fig. 3, created supplemental table of mean relabund for each species
</commit_message>
<xml_diff>
--- a/freq.xlsx
+++ b/freq.xlsx
@@ -380,6 +380,11 @@
       </c>
     </row>
     <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -387,7 +392,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D2">
@@ -395,6 +400,11 @@
       </c>
     </row>
     <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -402,7 +412,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D3">
@@ -410,6 +420,11 @@
       </c>
     </row>
     <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>caly</t>
@@ -417,7 +432,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D4">
@@ -425,6 +440,11 @@
       </c>
     </row>
     <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>caly</t>
@@ -432,7 +452,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D5">
@@ -440,6 +460,11 @@
       </c>
     </row>
     <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>coco</t>
@@ -447,7 +472,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D6">
@@ -455,6 +480,11 @@
       </c>
     </row>
     <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>coco</t>
@@ -462,7 +492,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D7">
@@ -470,6 +500,11 @@
       </c>
     </row>
     <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>dece</t>
@@ -477,7 +512,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D8">
@@ -485,6 +520,11 @@
       </c>
     </row>
     <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>disp</t>
@@ -492,7 +532,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D9">
@@ -500,6 +540,11 @@
       </c>
     </row>
     <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -507,7 +552,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D10">
@@ -515,6 +560,11 @@
       </c>
     </row>
     <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -522,7 +572,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D11">
@@ -530,6 +580,11 @@
       </c>
     </row>
     <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>epci</t>
@@ -537,7 +592,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D12">
@@ -545,6 +600,11 @@
       </c>
     </row>
     <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>glma</t>
@@ -552,7 +612,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D13">
@@ -560,6 +620,11 @@
       </c>
     </row>
     <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>glma</t>
@@ -567,7 +632,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D14">
@@ -575,6 +640,11 @@
       </c>
     </row>
     <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>isce</t>
@@ -582,7 +652,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D15">
@@ -590,6 +660,11 @@
       </c>
     </row>
     <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>juar</t>
@@ -597,7 +672,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D16">
@@ -605,6 +680,11 @@
       </c>
     </row>
     <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>juba</t>
@@ -612,7 +692,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D17">
@@ -620,14 +700,19 @@
       </c>
     </row>
     <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>jute</t>
+          <t>juge</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D18">
@@ -635,6 +720,11 @@
       </c>
     </row>
     <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>poasp</t>
@@ -642,7 +732,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D19">
@@ -650,6 +740,11 @@
       </c>
     </row>
     <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>popa</t>
@@ -657,7 +752,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D20">
@@ -665,6 +760,11 @@
       </c>
     </row>
     <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>popa</t>
@@ -672,7 +772,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D21">
@@ -680,6 +780,11 @@
       </c>
     </row>
     <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>sade</t>
@@ -687,7 +792,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D22">
@@ -695,6 +800,11 @@
       </c>
     </row>
     <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>sade</t>
@@ -702,7 +812,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D23">
@@ -710,6 +820,11 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>spca</t>
@@ -717,7 +832,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D24">
@@ -725,6 +840,11 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>spca</t>
@@ -732,7 +852,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D25">
@@ -740,6 +860,11 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>sysu</t>
@@ -747,7 +872,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D26">
@@ -755,6 +880,11 @@
       </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Grubbed</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>trma</t>
@@ -762,7 +892,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D27">
@@ -770,6 +900,12 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -777,7 +913,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D28">
@@ -785,6 +921,12 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>caly</t>
@@ -792,7 +934,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D29">
@@ -800,6 +942,12 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>caly</t>
@@ -807,7 +955,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D30">
@@ -815,6 +963,12 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>coco</t>
@@ -822,7 +976,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D31">
@@ -830,6 +984,12 @@
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>coco</t>
@@ -837,7 +997,7 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D32">
@@ -845,6 +1005,12 @@
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>dece</t>
@@ -852,7 +1018,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D33">
@@ -860,6 +1026,12 @@
       </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>dece</t>
@@ -867,7 +1039,7 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D34">
@@ -875,6 +1047,12 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>disp</t>
@@ -882,7 +1060,7 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D35">
@@ -890,6 +1068,12 @@
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -897,7 +1081,7 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D36">
@@ -905,6 +1089,12 @@
       </c>
     </row>
     <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -912,7 +1102,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D37">
@@ -920,6 +1110,12 @@
       </c>
     </row>
     <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>glma</t>
@@ -927,7 +1123,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D38">
@@ -935,6 +1131,12 @@
       </c>
     </row>
     <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>glma</t>
@@ -942,7 +1144,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D39">
@@ -950,6 +1152,12 @@
       </c>
     </row>
     <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr">
         <is>
           <t>juba</t>
@@ -957,7 +1165,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D40">
@@ -965,6 +1173,12 @@
       </c>
     </row>
     <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
           <t>juba</t>
@@ -972,7 +1186,7 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D41">
@@ -980,14 +1194,20 @@
       </c>
     </row>
     <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>jute</t>
+          <t>juge</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D42">
@@ -995,6 +1215,12 @@
       </c>
     </row>
     <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B43" t="inlineStr">
         <is>
           <t>sade</t>
@@ -1002,7 +1228,7 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D43">
@@ -1010,6 +1236,12 @@
       </c>
     </row>
     <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>sade</t>
@@ -1017,7 +1249,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D44">
@@ -1025,6 +1257,12 @@
       </c>
     </row>
     <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>spca</t>
@@ -1032,7 +1270,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D45">
@@ -1040,6 +1278,12 @@
       </c>
     </row>
     <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>spca</t>
@@ -1047,7 +1291,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D46">
@@ -1055,6 +1299,12 @@
       </c>
     </row>
     <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 1 year</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>trma</t>
@@ -1062,7 +1312,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D47">
@@ -1070,6 +1320,12 @@
       </c>
     </row>
     <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -1077,7 +1333,7 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D48">
@@ -1085,6 +1341,12 @@
       </c>
     </row>
     <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -1092,7 +1354,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D49">
@@ -1100,6 +1362,12 @@
       </c>
     </row>
     <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>caly</t>
@@ -1107,7 +1375,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D50">
@@ -1115,6 +1383,12 @@
       </c>
     </row>
     <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>caly</t>
@@ -1122,7 +1396,7 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D51">
@@ -1130,6 +1404,12 @@
       </c>
     </row>
     <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>coco</t>
@@ -1137,7 +1417,7 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D52">
@@ -1145,6 +1425,12 @@
       </c>
     </row>
     <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -1152,7 +1438,7 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D53">
@@ -1160,6 +1446,12 @@
       </c>
     </row>
     <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr">
         <is>
           <t>glma</t>
@@ -1167,7 +1459,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D54">
@@ -1175,6 +1467,12 @@
       </c>
     </row>
     <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B55" t="inlineStr">
         <is>
           <t>glma</t>
@@ -1182,7 +1480,7 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D55">
@@ -1190,6 +1488,12 @@
       </c>
     </row>
     <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B56" t="inlineStr">
         <is>
           <t>juba</t>
@@ -1197,7 +1501,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D56">
@@ -1205,6 +1509,12 @@
       </c>
     </row>
     <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>juba</t>
@@ -1212,7 +1522,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D57">
@@ -1220,6 +1530,12 @@
       </c>
     </row>
     <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B58" t="inlineStr">
         <is>
           <t>popa</t>
@@ -1227,7 +1543,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D58">
@@ -1235,6 +1551,12 @@
       </c>
     </row>
     <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B59" t="inlineStr">
         <is>
           <t>popa</t>
@@ -1242,7 +1564,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D59">
@@ -1250,6 +1572,12 @@
       </c>
     </row>
     <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B60" t="inlineStr">
         <is>
           <t>spca</t>
@@ -1257,7 +1585,7 @@
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D60">
@@ -1265,6 +1593,12 @@
       </c>
     </row>
     <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B61" t="inlineStr">
         <is>
           <t>trma</t>
@@ -1272,7 +1606,7 @@
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D61">
@@ -1280,6 +1614,12 @@
       </c>
     </row>
     <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Heavily Grazed, 
+Exclosed 10 years</t>
+        </is>
+      </c>
       <c r="B62" t="inlineStr">
         <is>
           <t>trma</t>
@@ -1287,7 +1627,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D62">
@@ -1295,6 +1635,11 @@
       </c>
     </row>
     <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B63" t="inlineStr">
         <is>
           <t>achmi</t>
@@ -1302,7 +1647,7 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D63">
@@ -1310,6 +1655,11 @@
       </c>
     </row>
     <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B64" t="inlineStr">
         <is>
           <t>agre</t>
@@ -1317,7 +1667,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D64">
@@ -1325,6 +1675,11 @@
       </c>
     </row>
     <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B65" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -1332,7 +1687,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D65">
@@ -1340,6 +1695,11 @@
       </c>
     </row>
     <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B66" t="inlineStr">
         <is>
           <t>agsp</t>
@@ -1347,7 +1707,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D66">
@@ -1355,6 +1715,11 @@
       </c>
     </row>
     <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B67" t="inlineStr">
         <is>
           <t>atpa</t>
@@ -1362,7 +1727,7 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D67">
@@ -1370,6 +1735,11 @@
       </c>
     </row>
     <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B68" t="inlineStr">
         <is>
           <t>caly</t>
@@ -1377,7 +1747,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D68">
@@ -1385,6 +1755,11 @@
       </c>
     </row>
     <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B69" t="inlineStr">
         <is>
           <t>caly</t>
@@ -1392,7 +1767,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D69">
@@ -1400,6 +1775,11 @@
       </c>
     </row>
     <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>coco</t>
@@ -1407,7 +1787,7 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D70">
@@ -1415,6 +1795,11 @@
       </c>
     </row>
     <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B71" t="inlineStr">
         <is>
           <t>dece</t>
@@ -1422,7 +1807,7 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D71">
@@ -1430,6 +1815,11 @@
       </c>
     </row>
     <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B72" t="inlineStr">
         <is>
           <t>disp</t>
@@ -1437,7 +1827,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D72">
@@ -1445,6 +1835,11 @@
       </c>
     </row>
     <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -1452,7 +1847,7 @@
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D73">
@@ -1460,6 +1855,11 @@
       </c>
     </row>
     <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B74" t="inlineStr">
         <is>
           <t>elpar</t>
@@ -1467,7 +1867,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D74">
@@ -1475,6 +1875,11 @@
       </c>
     </row>
     <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B75" t="inlineStr">
         <is>
           <t>epci</t>
@@ -1482,7 +1887,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D75">
@@ -1490,6 +1895,11 @@
       </c>
     </row>
     <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B76" t="inlineStr">
         <is>
           <t>epgl</t>
@@ -1497,7 +1907,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D76">
@@ -1505,6 +1915,11 @@
       </c>
     </row>
     <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B77" t="inlineStr">
         <is>
           <t>glma</t>
@@ -1512,7 +1927,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D77">
@@ -1520,6 +1935,11 @@
       </c>
     </row>
     <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B78" t="inlineStr">
         <is>
           <t>glma</t>
@@ -1527,7 +1947,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D78">
@@ -1535,6 +1955,11 @@
       </c>
     </row>
     <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B79" t="inlineStr">
         <is>
           <t>grsp</t>
@@ -1542,7 +1967,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D79">
@@ -1550,6 +1975,11 @@
       </c>
     </row>
     <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B80" t="inlineStr">
         <is>
           <t>isce</t>
@@ -1557,7 +1987,7 @@
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D80">
@@ -1565,6 +1995,11 @@
       </c>
     </row>
     <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B81" t="inlineStr">
         <is>
           <t>juar</t>
@@ -1572,7 +2007,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D81">
@@ -1580,6 +2015,11 @@
       </c>
     </row>
     <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B82" t="inlineStr">
         <is>
           <t>juba</t>
@@ -1587,7 +2027,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D82">
@@ -1595,6 +2035,11 @@
       </c>
     </row>
     <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B83" t="inlineStr">
         <is>
           <t>juba</t>
@@ -1602,7 +2047,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D83">
@@ -1610,6 +2055,11 @@
       </c>
     </row>
     <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B84" t="inlineStr">
         <is>
           <t>juen</t>
@@ -1617,7 +2067,7 @@
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D84">
@@ -1625,14 +2075,19 @@
       </c>
     </row>
     <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>jute</t>
+          <t>juge</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D85">
@@ -1640,6 +2095,11 @@
       </c>
     </row>
     <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B86" t="inlineStr">
         <is>
           <t>popa</t>
@@ -1647,7 +2107,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D86">
@@ -1655,6 +2115,11 @@
       </c>
     </row>
     <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B87" t="inlineStr">
         <is>
           <t>popa</t>
@@ -1662,7 +2127,7 @@
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D87">
@@ -1670,6 +2135,11 @@
       </c>
     </row>
     <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B88" t="inlineStr">
         <is>
           <t>sade</t>
@@ -1677,7 +2147,7 @@
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D88">
@@ -1685,6 +2155,11 @@
       </c>
     </row>
     <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B89" t="inlineStr">
         <is>
           <t>spca</t>
@@ -1692,7 +2167,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D89">
@@ -1700,6 +2175,11 @@
       </c>
     </row>
     <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
           <t>spca</t>
@@ -1707,7 +2187,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D90">
@@ -1715,6 +2195,11 @@
       </c>
     </row>
     <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B91" t="inlineStr">
         <is>
           <t>sysu</t>
@@ -1722,7 +2207,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Surface seed bank</t>
+          <t>seed</t>
         </is>
       </c>
       <c r="D91">
@@ -1730,6 +2215,11 @@
       </c>
     </row>
     <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B92" t="inlineStr">
         <is>
           <t>sysu</t>
@@ -1737,7 +2227,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D92">
@@ -1745,6 +2235,11 @@
       </c>
     </row>
     <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B93" t="inlineStr">
         <is>
           <t>trma</t>
@@ -1752,7 +2247,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D93">
@@ -1760,6 +2255,11 @@
       </c>
     </row>
     <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Undisturbed</t>
+        </is>
+      </c>
       <c r="B94" t="inlineStr">
         <is>
           <t>trwo</t>
@@ -1767,7 +2267,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Above-ground vegetation</t>
+          <t>veg</t>
         </is>
       </c>
       <c r="D94">

</xml_diff>